<commit_message>
small edit in graphs
</commit_message>
<xml_diff>
--- a/data/elec_price/dereg_year.xlsx
+++ b/data/elec_price/dereg_year.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orshahar/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orshahar/Desktop/School/causality_analysis/data/elec_price/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78DE6DD9-8CAC-0C4B-91B8-3CD1CA400ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51706695-CDF9-3342-919A-7873AA53C363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{81D2186B-7C75-CB49-9F1A-DE1940F1D16B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>IL</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>CT</t>
+  </si>
+  <si>
+    <t>CA</t>
   </si>
 </sst>
 </file>
@@ -485,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98825382-052F-4C49-9E31-84DC33C261CC}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,79 +506,79 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2">
-        <v>1998</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>1997</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>2000</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>1998</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>1997</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>1998</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>1999</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>1999</v>
@@ -583,23 +586,23 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>1997</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>1999</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>1999</v>
@@ -607,31 +610,39 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15">
-        <v>1996</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>2002</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>1999</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B42">
-    <sortCondition ref="A2:A42"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B43">
+    <sortCondition ref="A3:A43"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>